<commit_message>
Fixed the scheduler output
</commit_message>
<xml_diff>
--- a/static/excel_templates/workload_template.xlsx
+++ b/static/excel_templates/workload_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IntelliSched-An-AI-Assisted-Instructor-Student-Scheduling-System\static\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0243C0C0-5C81-4C27-8ED4-C5BFF13D4433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090A306F-95BE-450C-9240-AD6AAC7DB7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E1F356F-A708-4270-8126-3C159C96E70A}"/>
   </bookViews>
@@ -193,106 +193,106 @@
     <t>Instructional Functions:</t>
   </si>
   <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>OVERLOAD/PART-TIME</t>
+  </si>
+  <si>
+    <t>header_faculty</t>
+  </si>
+  <si>
+    <t>header_semester</t>
+  </si>
+  <si>
+    <t>header_rank</t>
+  </si>
+  <si>
+    <t>header_sy</t>
+  </si>
+  <si>
+    <t>header_college</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>lec</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>students</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>inv_admin</t>
+  </si>
+  <si>
+    <t>inv_extension</t>
+  </si>
+  <si>
+    <t>inv_consultation</t>
+  </si>
+  <si>
+    <t>inv_classes</t>
+  </si>
+  <si>
+    <t>inv_total</t>
+  </si>
+  <si>
+    <t>sig_faculty</t>
+  </si>
+  <si>
+    <t>sig_dept_head</t>
+  </si>
+  <si>
+    <t>sig_dean</t>
+  </si>
+  <si>
+    <t>sig_vp</t>
+  </si>
+  <si>
+    <t>sig_president</t>
+  </si>
+  <si>
+    <t>Department Head</t>
+  </si>
+  <si>
+    <t>Dean, School of Engineering</t>
+  </si>
+  <si>
+    <t>Vice-President for Academic Affairs</t>
+  </si>
+  <si>
+    <t>University President</t>
+  </si>
+  <si>
+    <t>inv_research</t>
+  </si>
+  <si>
+    <t>inv_others</t>
+  </si>
+  <si>
     <t>Others (Please Specify):</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t>OVERLOAD/PART-TIME</t>
-  </si>
-  <si>
-    <t>header_faculty</t>
-  </si>
-  <si>
-    <t>header_semester</t>
-  </si>
-  <si>
-    <t>header_rank</t>
-  </si>
-  <si>
-    <t>header_sy</t>
-  </si>
-  <si>
-    <t>header_college</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>days</t>
-  </si>
-  <si>
-    <t>lec</t>
-  </si>
-  <si>
-    <t>lab</t>
-  </si>
-  <si>
-    <t>students</t>
-  </si>
-  <si>
-    <t>room</t>
-  </si>
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>inv_admin</t>
-  </si>
-  <si>
-    <t>inv_extension</t>
-  </si>
-  <si>
-    <t>inv_consultation</t>
-  </si>
-  <si>
-    <t>inv_classes</t>
-  </si>
-  <si>
-    <t>inv_total</t>
-  </si>
-  <si>
-    <t>sig_faculty</t>
-  </si>
-  <si>
-    <t>sig_dept_head</t>
-  </si>
-  <si>
-    <t>sig_dean</t>
-  </si>
-  <si>
-    <t>sig_vp</t>
-  </si>
-  <si>
-    <t>sig_president</t>
-  </si>
-  <si>
-    <t>Department Head</t>
-  </si>
-  <si>
-    <t>Dean, School of Engineering</t>
-  </si>
-  <si>
-    <t>Vice-President for Academic Affairs</t>
-  </si>
-  <si>
-    <t>University President</t>
-  </si>
-  <si>
-    <t>inv_research</t>
-  </si>
-  <si>
-    <t>inv_others</t>
   </si>
 </sst>
 </file>
@@ -600,116 +600,116 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,151 +1113,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="26" t="s">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
       <c r="P3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="54" t="s">
+      <c r="Q3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="54"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
       <c r="P4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="55" t="s">
+      <c r="Q4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="54"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
       <c r="P5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="54" t="s">
+      <c r="Q5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="54"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="B7" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1271,21 +1271,21 @@
       <c r="P7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" s="50"/>
+      <c r="Q7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="26"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="B8" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1299,21 +1299,21 @@
       <c r="P8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="R8" s="50"/>
+      <c r="Q8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="26"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="B9" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1327,171 +1327,171 @@
       <c r="P9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27" t="s">
+      <c r="I12" s="29"/>
+      <c r="J12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27" t="s">
+      <c r="K12" s="29"/>
+      <c r="L12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27" t="s">
+      <c r="N12" s="29"/>
+      <c r="O12" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="27" t="s">
+      <c r="Q12" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="27"/>
+      <c r="R12" s="29"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
       <c r="M13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="47" t="s">
+      <c r="K14" s="21"/>
+      <c r="L14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q14" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="R14" s="26"/>
+      <c r="R14" s="21"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="35" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="35">
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="33">
         <f>SUM(H14:I14)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="33"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="6">
         <f>SUM(M14:M14)</f>
         <v>0</v>
@@ -1500,36 +1500,36 @@
         <f>SUM(N14:N14)</f>
         <v>0</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="31">
         <f>SUM(O14:O14)</f>
         <v>0</v>
       </c>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="36"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="34"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="39">
+      <c r="A16" s="41"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="37">
         <f>SUM(M15:N15)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="40"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="36"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1552,147 +1552,147 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="A18" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27" t="s">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27" t="s">
+      <c r="I19" s="29"/>
+      <c r="J19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27" t="s">
+      <c r="K19" s="29"/>
+      <c r="L19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="M19" s="27" t="s">
+      <c r="M19" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27" t="s">
+      <c r="N19" s="29"/>
+      <c r="O19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P19" s="27" t="s">
+      <c r="P19" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Q19" s="27" t="s">
+      <c r="Q19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="R19" s="27"/>
+      <c r="R19" s="29"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
       <c r="M20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="28" t="s">
+      <c r="I21" s="46"/>
+      <c r="J21" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31" t="s">
+      <c r="K21" s="48"/>
+      <c r="L21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="32"/>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="Q21" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="R21" s="30"/>
+      <c r="R21" s="46"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27">
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29">
         <f>SUM(H21:I21)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
       <c r="M22" s="6">
         <f>SUM(M21:M21)</f>
         <v>0</v>
@@ -1701,45 +1701,45 @@
         <f>SUM(N21:N21)</f>
         <v>0</v>
       </c>
-      <c r="O22" s="27">
+      <c r="O22" s="29">
         <f>SUM(O21:O21)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27">
+      <c r="A23" s="21"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29">
         <f>SUM(M22:N22)</f>
         <v>0</v>
       </c>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
     </row>
     <row r="24" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="8"/>
@@ -1752,19 +1752,19 @@
       <c r="O24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="P24" s="20" t="s">
+      <c r="P24" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>31</v>
@@ -1780,17 +1780,17 @@
       <c r="M25" s="8"/>
       <c r="N25" s="10"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="21"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>31</v>
@@ -1800,27 +1800,27 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="23" t="s">
+      <c r="J26" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="23"/>
+      <c r="K26" s="50"/>
       <c r="L26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>31</v>
@@ -1830,12 +1830,12 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="K27" s="23"/>
+      <c r="K27" s="50"/>
       <c r="L27" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
@@ -1845,10 +1845,10 @@
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="9"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -1867,12 +1867,12 @@
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>31</v>
@@ -1893,12 +1893,12 @@
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="21"/>
+      <c r="A30" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="49"/>
       <c r="C30" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>31</v>
@@ -1959,109 +1959,110 @@
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="51"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="24" t="s">
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="24" t="s">
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="24" t="s">
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="24" t="s">
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="52"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="25" t="s">
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="25" t="s">
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="25" t="s">
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
+      <c r="Q34" s="52"/>
+      <c r="R34" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="C1:R2"/>
-    <mergeCell ref="C3:O5"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:R13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="P25:R26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:G23"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:R23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:R20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:N19"/>
     <mergeCell ref="P15:P16"/>
     <mergeCell ref="Q15:R16"/>
     <mergeCell ref="M16:N16"/>
@@ -2075,49 +2076,48 @@
     <mergeCell ref="J15:K16"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="O15:O16"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:R23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:R20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:G23"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="J22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="P25:R26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:R13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="C1:R2"/>
+    <mergeCell ref="C3:O5"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added a semester selector and improved workload mport/export
</commit_message>
<xml_diff>
--- a/static/excel_templates/workload_template.xlsx
+++ b/static/excel_templates/workload_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IntelliSched-An-AI-Assisted-Instructor-Student-Scheduling-System\static\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090A306F-95BE-450C-9240-AD6AAC7DB7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73DCC5C-53D2-4D56-BC42-B8884E75030C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E1F356F-A708-4270-8126-3C159C96E70A}"/>
   </bookViews>
@@ -256,9 +256,6 @@
     <t>inv_classes</t>
   </si>
   <si>
-    <t>inv_total</t>
-  </si>
-  <si>
     <t>sig_faculty</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>Others (Please Specify):</t>
+  </si>
+  <si>
+    <t>inv_preps</t>
   </si>
 </sst>
 </file>
@@ -600,13 +600,106 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -617,99 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,151 +1113,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="22" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
       <c r="P3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="54"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
       <c r="P4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="23"/>
+      <c r="R4" s="54"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
       <c r="P5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="Q5" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="23"/>
+      <c r="R5" s="54"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1271,21 +1271,21 @@
       <c r="P7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="26"/>
+      <c r="R7" s="48"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1299,21 +1299,21 @@
       <c r="P8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="26" t="s">
+      <c r="Q8" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="26"/>
+      <c r="R8" s="48"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1327,133 +1327,133 @@
       <c r="P9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29" t="s">
+      <c r="I12" s="27"/>
+      <c r="J12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29" t="s">
+      <c r="K12" s="27"/>
+      <c r="L12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29" t="s">
+      <c r="N12" s="27"/>
+      <c r="O12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="29" t="s">
+      <c r="Q12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="29"/>
+      <c r="R12" s="27"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
       <c r="M13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="30" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="21"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="1" t="s">
         <v>49</v>
       </c>
@@ -1469,29 +1469,29 @@
       <c r="P14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="Q14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="R14" s="21"/>
+      <c r="R14" s="26"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="33">
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35">
         <f>SUM(H14:I14)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="31"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="33"/>
       <c r="M15" s="6">
         <f>SUM(M14:M14)</f>
         <v>0</v>
@@ -1500,36 +1500,36 @@
         <f>SUM(N14:N14)</f>
         <v>0</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="33">
         <f>SUM(O14:O14)</f>
         <v>0</v>
       </c>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="34"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="36"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="37">
+      <c r="A16" s="44"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="39">
         <f>SUM(M15:N15)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="38"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="38"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1552,109 +1552,109 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29" t="s">
+      <c r="I19" s="27"/>
+      <c r="J19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29" t="s">
+      <c r="K19" s="27"/>
+      <c r="L19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29" t="s">
+      <c r="N19" s="27"/>
+      <c r="O19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P19" s="29" t="s">
+      <c r="P19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="Q19" s="29" t="s">
+      <c r="Q19" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R19" s="29"/>
+      <c r="R19" s="27"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
       <c r="M20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="44" t="s">
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="46"/>
-      <c r="J21" s="47" t="s">
+      <c r="I21" s="30"/>
+      <c r="J21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="K21" s="48"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="1" t="s">
         <v>49</v>
       </c>
@@ -1670,29 +1670,29 @@
       <c r="P21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R21" s="46"/>
+      <c r="R21" s="30"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="29" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29">
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27">
         <f>SUM(H21:I21)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
       <c r="M22" s="6">
         <f>SUM(M21:M21)</f>
         <v>0</v>
@@ -1701,45 +1701,45 @@
         <f>SUM(N21:N21)</f>
         <v>0</v>
       </c>
-      <c r="O22" s="29">
+      <c r="O22" s="27">
         <f>SUM(O21:O21)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29">
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27">
         <f>SUM(M22:N22)</f>
         <v>0</v>
       </c>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
     </row>
     <row r="24" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="8"/>
@@ -1752,17 +1752,17 @@
       <c r="O24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="P24" s="54" t="s">
+      <c r="P24" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="12" t="s">
         <v>55</v>
       </c>
@@ -1780,17 +1780,17 @@
       <c r="M25" s="8"/>
       <c r="N25" s="10"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="49"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>31</v>
@@ -1800,25 +1800,25 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="50"/>
+      <c r="K26" s="23"/>
       <c r="L26" s="12" t="s">
         <v>58</v>
       </c>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="49"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="18" t="s">
         <v>56</v>
       </c>
@@ -1830,12 +1830,12 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K27" s="50"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
@@ -1845,10 +1845,10 @@
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="49"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="9"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -1867,10 +1867,10 @@
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="12" t="s">
         <v>57</v>
       </c>
@@ -1893,12 +1893,12 @@
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="49"/>
+      <c r="A30" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="21"/>
       <c r="C30" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>31</v>
@@ -1959,110 +1959,109 @@
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="51" t="s">
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="51" t="s">
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="51" t="s">
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="51" t="s">
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="51"/>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="52" t="s">
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="52" t="s">
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="52" t="s">
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="P25:R26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:G23"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="J22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:R23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:R20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="C1:R2"/>
+    <mergeCell ref="C3:O5"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:R13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="Q14:R14"/>
     <mergeCell ref="P15:P16"/>
     <mergeCell ref="Q15:R16"/>
     <mergeCell ref="M16:N16"/>
@@ -2076,48 +2075,49 @@
     <mergeCell ref="J15:K16"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="O15:O16"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:R13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="C1:R2"/>
-    <mergeCell ref="C3:O5"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:R23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:R20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:G23"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="P25:R26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="J26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>